<commit_message>
filling missing quarters for keler, omi, kdpw, lchsa, lchlts, ice nl, ice europe
</commit_message>
<xml_diff>
--- a/data/full_data/bme clearing.xlsx
+++ b/data/full_data/bme clearing.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>CCP</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Q2-2016</t>
+  </si>
+  <si>
+    <t>Q1-2016</t>
+  </si>
+  <si>
+    <t>Q4-2015</t>
   </si>
   <si>
     <t>Q4-2017</t>
@@ -495,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC46"/>
+  <dimension ref="A1:AC56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2826,17 +2832,17 @@
       <c r="E27" t="n">
         <v>2000000</v>
       </c>
-      <c r="F27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G27" t="s">
-        <v>31</v>
+      <c r="F27" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2000000</v>
       </c>
       <c r="H27" t="n">
-        <v>341050000</v>
+        <v>78950000</v>
       </c>
       <c r="I27" t="n">
-        <v>341050000</v>
+        <v>78950000</v>
       </c>
       <c r="J27" t="s">
         <v>31</v>
@@ -2845,31 +2851,31 @@
         <v>4000000</v>
       </c>
       <c r="L27" t="n">
-        <v>682100000</v>
+        <v>157900000</v>
       </c>
       <c r="M27" t="n">
-        <v>682100000</v>
-      </c>
-      <c r="N27" t="n">
-        <v>341050000</v>
+        <v>157900000</v>
+      </c>
+      <c r="N27" t="s">
+        <v>31</v>
       </c>
       <c r="O27" t="n">
-        <v>415901572.28</v>
+        <v>222834996.24</v>
       </c>
       <c r="P27" t="n">
-        <v>281700432.0429804</v>
+        <v>118573439.4034119</v>
       </c>
       <c r="Q27" t="n">
-        <v>1231882238.22</v>
+        <v>840207830.5170077</v>
       </c>
       <c r="R27" t="n">
-        <v>2198469355.610001</v>
+        <v>1920399210.684806</v>
       </c>
       <c r="S27" t="n">
-        <v>2513224563.499913</v>
+        <v>2213341110.764022</v>
       </c>
       <c r="T27" t="n">
-        <v>2349927191.849818</v>
+        <v>2018260014.626199</v>
       </c>
       <c r="U27" t="n">
         <v>38</v>
@@ -2877,26 +2883,26 @@
       <c r="V27" t="n">
         <v>0</v>
       </c>
-      <c r="W27" t="n">
-        <v>0</v>
+      <c r="W27" t="s">
+        <v>31</v>
       </c>
       <c r="X27" t="n">
-        <v>42775</v>
+        <v>59604</v>
       </c>
       <c r="Y27" t="n">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="Z27" t="n">
         <v>0</v>
       </c>
       <c r="AA27" t="n">
-        <v>3412149206.349206</v>
+        <v>0</v>
       </c>
       <c r="AB27" t="n">
         <v>0</v>
       </c>
       <c r="AC27" t="n">
-        <v>16735799835.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:29">
@@ -2915,17 +2921,17 @@
       <c r="E28" t="n">
         <v>1000000</v>
       </c>
-      <c r="F28" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" t="s">
-        <v>31</v>
+      <c r="F28" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1000000</v>
       </c>
       <c r="H28" t="n">
-        <v>28000000</v>
+        <v>30000000</v>
       </c>
       <c r="I28" t="n">
-        <v>28000000</v>
+        <v>30000000</v>
       </c>
       <c r="J28" t="s">
         <v>31</v>
@@ -2934,58 +2940,58 @@
         <v>2000000</v>
       </c>
       <c r="L28" t="n">
-        <v>56000000</v>
+        <v>60000000</v>
       </c>
       <c r="M28" t="n">
-        <v>56000000</v>
-      </c>
-      <c r="N28" t="n">
-        <v>28000000</v>
+        <v>60000000</v>
+      </c>
+      <c r="N28" t="s">
+        <v>31</v>
       </c>
       <c r="O28" t="n">
-        <v>83624817.22999999</v>
+        <v>291087155.92</v>
       </c>
       <c r="P28" t="n">
-        <v>22918862.46031372</v>
+        <v>73110715.03809799</v>
       </c>
       <c r="Q28" t="n">
-        <v>2116247.92</v>
+        <v>0</v>
       </c>
       <c r="R28" t="n">
-        <v>1291836830.6</v>
+        <v>1578057124.0158</v>
       </c>
       <c r="S28" t="n">
-        <v>1775456383.446402</v>
+        <v>1861662116.051824</v>
       </c>
       <c r="T28" t="n">
-        <v>1730858382.008108</v>
+        <v>1831863674.503802</v>
       </c>
       <c r="U28" t="n">
         <v>0</v>
       </c>
       <c r="V28" t="n">
-        <v>28</v>
-      </c>
-      <c r="W28" t="n">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="W28" t="s">
+        <v>31</v>
       </c>
       <c r="X28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z28" t="n">
         <v>0</v>
       </c>
       <c r="AA28" t="n">
-        <v>2147561134.778922</v>
+        <v>0</v>
       </c>
       <c r="AB28" t="n">
         <v>0</v>
       </c>
       <c r="AC28" t="n">
-        <v>17868539938.52748</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:29">
@@ -3004,17 +3010,17 @@
       <c r="E29" t="n">
         <v>500000</v>
       </c>
-      <c r="F29" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" t="s">
-        <v>31</v>
+      <c r="F29" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G29" t="n">
+        <v>500000</v>
       </c>
       <c r="H29" t="n">
-        <v>13200000</v>
+        <v>5700000</v>
       </c>
       <c r="I29" t="n">
-        <v>13200000</v>
+        <v>5700000</v>
       </c>
       <c r="J29" t="s">
         <v>31</v>
@@ -3023,58 +3029,58 @@
         <v>1000000</v>
       </c>
       <c r="L29" t="n">
-        <v>26400000</v>
+        <v>11400000</v>
       </c>
       <c r="M29" t="n">
-        <v>26400000</v>
-      </c>
-      <c r="N29" t="n">
-        <v>13200000</v>
+        <v>11400000</v>
+      </c>
+      <c r="N29" t="s">
+        <v>31</v>
       </c>
       <c r="O29" t="n">
-        <v>16185622.88</v>
+        <v>12812004.39</v>
       </c>
       <c r="P29" t="n">
-        <v>11314466.51141176</v>
+        <v>5657893.462745098</v>
       </c>
       <c r="Q29" t="n">
-        <v>79033552.61</v>
+        <v>27213453.61452016</v>
       </c>
       <c r="R29" t="n">
-        <v>79033552.61</v>
+        <v>69132037.96939412</v>
       </c>
       <c r="S29" t="n">
-        <v>78909861.05337371</v>
+        <v>70193531.93000001</v>
       </c>
       <c r="T29" t="n">
-        <v>78732192.92559727</v>
+        <v>70193531.93000001</v>
       </c>
       <c r="U29" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V29" t="n">
         <v>0</v>
       </c>
-      <c r="W29" t="n">
-        <v>0</v>
+      <c r="W29" t="s">
+        <v>31</v>
       </c>
       <c r="X29" t="n">
-        <v>168</v>
+        <v>104</v>
       </c>
       <c r="Y29" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Z29" t="n">
         <v>0</v>
       </c>
       <c r="AA29" t="n">
-        <v>2627670.127619048</v>
+        <v>0</v>
       </c>
       <c r="AB29" t="n">
         <v>0</v>
       </c>
       <c r="AC29" t="n">
-        <v>490426526.1749998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:29">
@@ -3093,11 +3099,11 @@
       <c r="E30" t="n">
         <v>1000000</v>
       </c>
-      <c r="F30" t="s">
-        <v>31</v>
-      </c>
-      <c r="G30" t="s">
-        <v>31</v>
+      <c r="F30" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1000000</v>
       </c>
       <c r="H30" t="n">
         <v>8000000</v>
@@ -3117,35 +3123,35 @@
       <c r="M30" t="n">
         <v>16000000</v>
       </c>
-      <c r="N30" t="n">
-        <v>8000000</v>
-      </c>
-      <c r="O30" t="n">
-        <v>15905959.9772</v>
-      </c>
-      <c r="P30" t="n">
-        <v>8481269.385170585</v>
+      <c r="N30" t="s">
+        <v>31</v>
+      </c>
+      <c r="O30" t="s">
+        <v>31</v>
+      </c>
+      <c r="P30" t="s">
+        <v>31</v>
       </c>
       <c r="Q30" t="n">
         <v>0</v>
       </c>
       <c r="R30" t="n">
-        <v>7959389.49</v>
+        <v>2105248.74</v>
       </c>
       <c r="S30" t="n">
-        <v>31962562.32236112</v>
+        <v>3941041.747800011</v>
       </c>
       <c r="T30" t="n">
-        <v>30198249.05959623</v>
+        <v>3931462.020000011</v>
       </c>
       <c r="U30" t="n">
         <v>0</v>
       </c>
       <c r="V30" t="n">
-        <v>9</v>
-      </c>
-      <c r="W30" t="n">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="W30" t="s">
+        <v>31</v>
       </c>
       <c r="X30" t="n">
         <v>0</v>
@@ -3154,13 +3160,13 @@
         <v>0</v>
       </c>
       <c r="Z30" t="n">
-        <v>24825396.82539682</v>
+        <v>0</v>
       </c>
       <c r="AA30" t="n">
         <v>0</v>
       </c>
       <c r="AB30" t="n">
-        <v>469913313.8699999</v>
+        <v>0</v>
       </c>
       <c r="AC30" t="n">
         <v>0</v>
@@ -3179,80 +3185,40 @@
       <c r="D31" t="s">
         <v>35</v>
       </c>
-      <c r="E31" t="n">
-        <v>1500000</v>
-      </c>
-      <c r="F31" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" t="n">
-        <v>88250000</v>
-      </c>
-      <c r="I31" t="n">
-        <v>88250000</v>
-      </c>
-      <c r="J31" t="s">
-        <v>31</v>
-      </c>
-      <c r="K31" t="n">
-        <v>3000000</v>
-      </c>
-      <c r="L31" t="n">
-        <v>176500000</v>
-      </c>
-      <c r="M31" t="n">
-        <v>176500000</v>
-      </c>
-      <c r="N31" t="n">
-        <v>88250000</v>
-      </c>
-      <c r="O31" t="n">
-        <v>749432256</v>
-      </c>
-      <c r="P31" t="n">
-        <v>127219022.2716863</v>
-      </c>
+      <c r="E31" t="s"/>
+      <c r="F31" t="s"/>
+      <c r="G31" t="s"/>
+      <c r="H31" t="s"/>
+      <c r="I31" t="s"/>
+      <c r="J31" t="s"/>
+      <c r="K31" t="s"/>
+      <c r="L31" t="s"/>
+      <c r="M31" t="s"/>
+      <c r="N31" t="s"/>
+      <c r="O31" t="s"/>
+      <c r="P31" t="s"/>
       <c r="Q31" t="n">
-        <v>198285453.89</v>
-      </c>
-      <c r="R31" t="n">
-        <v>202904762.5700001</v>
-      </c>
-      <c r="S31" t="n">
-        <v>424144037.7920223</v>
-      </c>
-      <c r="T31" t="n">
-        <v>404341742.3368806</v>
-      </c>
-      <c r="U31" t="n">
-        <v>28</v>
-      </c>
-      <c r="V31" t="n">
-        <v>0</v>
-      </c>
-      <c r="W31" t="n">
-        <v>0</v>
-      </c>
-      <c r="X31" t="n">
-        <v>258</v>
-      </c>
-      <c r="Y31" t="n">
-        <v>27</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R31" t="s"/>
+      <c r="S31" t="s"/>
+      <c r="T31" t="s"/>
+      <c r="U31" t="s"/>
+      <c r="V31" t="s"/>
+      <c r="W31" t="s"/>
+      <c r="X31" t="s"/>
+      <c r="Y31" t="s"/>
       <c r="Z31" t="n">
         <v>0</v>
       </c>
       <c r="AA31" t="n">
-        <v>4983780341.471429</v>
+        <v>0</v>
       </c>
       <c r="AB31" t="n">
         <v>0</v>
       </c>
       <c r="AC31" t="n">
-        <v>1835750898.48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:29">
@@ -3278,10 +3244,10 @@
         <v>31</v>
       </c>
       <c r="H32" t="n">
-        <v>65250000</v>
+        <v>96100000</v>
       </c>
       <c r="I32" t="n">
-        <v>65250000</v>
+        <v>96100000</v>
       </c>
       <c r="J32" t="s">
         <v>31</v>
@@ -3290,34 +3256,34 @@
         <v>4000000</v>
       </c>
       <c r="L32" t="n">
-        <v>130500000</v>
+        <v>192200000</v>
       </c>
       <c r="M32" t="n">
-        <v>130500000</v>
+        <v>192200000</v>
       </c>
       <c r="N32" t="s">
         <v>31</v>
       </c>
       <c r="O32" t="n">
-        <v>128575078.3</v>
+        <v>222834996.24</v>
       </c>
       <c r="P32" t="n">
-        <v>85784721.51953307</v>
+        <v>135810192.0306827</v>
       </c>
       <c r="Q32" t="n">
-        <v>944508985.3000001</v>
+        <v>854611946.8215443</v>
       </c>
       <c r="R32" t="n">
-        <v>1615585684.27</v>
+        <v>1953321605.093845</v>
       </c>
       <c r="S32" t="n">
-        <v>2122726809.248829</v>
+        <v>2281139692.317715</v>
       </c>
       <c r="T32" t="n">
-        <v>1919778423.562241</v>
+        <v>2056269298.302852</v>
       </c>
       <c r="U32" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="V32" t="n">
         <v>0</v>
@@ -3326,22 +3292,22 @@
         <v>31</v>
       </c>
       <c r="X32" t="n">
-        <v>76593</v>
+        <v>60734</v>
       </c>
       <c r="Y32" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="Z32" t="n">
         <v>0</v>
       </c>
       <c r="AA32" t="n">
-        <v>2526057656.25</v>
+        <v>0</v>
       </c>
       <c r="AB32" t="n">
         <v>0</v>
       </c>
       <c r="AC32" t="n">
-        <v>12295069331.51122</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:29">
@@ -3358,7 +3324,7 @@
         <v>32</v>
       </c>
       <c r="E33" t="n">
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="F33" t="s">
         <v>31</v>
@@ -3367,49 +3333,49 @@
         <v>31</v>
       </c>
       <c r="H33" t="n">
-        <v>29000000</v>
+        <v>30000000</v>
       </c>
       <c r="I33" t="n">
-        <v>29000000</v>
+        <v>30000000</v>
       </c>
       <c r="J33" t="s">
         <v>31</v>
       </c>
       <c r="K33" t="n">
-        <v>2000000</v>
+        <v>4000000</v>
       </c>
       <c r="L33" t="n">
-        <v>58000000</v>
+        <v>60000000</v>
       </c>
       <c r="M33" t="n">
-        <v>58000000</v>
+        <v>60000000</v>
       </c>
       <c r="N33" t="s">
         <v>31</v>
       </c>
       <c r="O33" t="n">
-        <v>77564196.22</v>
+        <v>99378423.58</v>
       </c>
       <c r="P33" t="n">
-        <v>33825150.34933851</v>
+        <v>37237208.9799008</v>
       </c>
       <c r="Q33" t="n">
         <v>0</v>
       </c>
       <c r="R33" t="n">
-        <v>1081511424.12</v>
+        <v>2256647352.978095</v>
       </c>
       <c r="S33" t="n">
-        <v>1633609837.239741</v>
+        <v>2584757201.494524</v>
       </c>
       <c r="T33" t="n">
-        <v>1601753380.477004</v>
+        <v>2530456609.43881</v>
       </c>
       <c r="U33" t="n">
         <v>0</v>
       </c>
       <c r="V33" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="W33" t="s">
         <v>31</v>
@@ -3424,13 +3390,13 @@
         <v>0</v>
       </c>
       <c r="AA33" t="n">
-        <v>3018566648.816501</v>
+        <v>0</v>
       </c>
       <c r="AB33" t="n">
         <v>0</v>
       </c>
       <c r="AC33" t="n">
-        <v>17203359798.564</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:29">
@@ -3447,7 +3413,7 @@
         <v>33</v>
       </c>
       <c r="E34" t="n">
-        <v>500000</v>
+        <v>1000000</v>
       </c>
       <c r="F34" t="s">
         <v>31</v>
@@ -3456,46 +3422,46 @@
         <v>31</v>
       </c>
       <c r="H34" t="n">
-        <v>10000000</v>
+        <v>5550000</v>
       </c>
       <c r="I34" t="n">
-        <v>10000000</v>
+        <v>5550000</v>
       </c>
       <c r="J34" t="s">
         <v>31</v>
       </c>
       <c r="K34" t="n">
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="L34" t="n">
-        <v>20000000</v>
+        <v>11100000</v>
       </c>
       <c r="M34" t="n">
-        <v>20000000</v>
+        <v>11100000</v>
       </c>
       <c r="N34" t="s">
         <v>31</v>
       </c>
       <c r="O34" t="n">
-        <v>21539150.61</v>
+        <v>10729349.12</v>
       </c>
       <c r="P34" t="n">
-        <v>12919611.23412452</v>
+        <v>6310574.326184743</v>
       </c>
       <c r="Q34" t="n">
-        <v>60522636.47</v>
+        <v>21045958.57995747</v>
       </c>
       <c r="R34" t="n">
-        <v>61018440.4</v>
+        <v>53464364.65806031</v>
       </c>
       <c r="S34" t="n">
-        <v>67315060.94766967</v>
+        <v>65556677.27834146</v>
       </c>
       <c r="T34" t="n">
-        <v>66250545.85192169</v>
+        <v>65556677.27834146</v>
       </c>
       <c r="U34" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V34" t="n">
         <v>0</v>
@@ -3504,22 +3470,22 @@
         <v>31</v>
       </c>
       <c r="X34" t="n">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="Y34" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Z34" t="n">
         <v>0</v>
       </c>
       <c r="AA34" t="n">
-        <v>4910347.617656251</v>
+        <v>0</v>
       </c>
       <c r="AB34" t="n">
         <v>0</v>
       </c>
       <c r="AC34" t="n">
-        <v>441979282.6799994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:29">
@@ -3545,10 +3511,10 @@
         <v>31</v>
       </c>
       <c r="H35" t="n">
-        <v>19700000</v>
+        <v>6000000</v>
       </c>
       <c r="I35" t="n">
-        <v>19700000</v>
+        <v>6000000</v>
       </c>
       <c r="J35" t="s">
         <v>31</v>
@@ -3557,37 +3523,37 @@
         <v>2000000</v>
       </c>
       <c r="L35" t="n">
-        <v>39400000</v>
+        <v>12000000</v>
       </c>
       <c r="M35" t="n">
-        <v>39400000</v>
+        <v>12000000</v>
       </c>
       <c r="N35" t="s">
         <v>31</v>
       </c>
-      <c r="O35" t="n">
-        <v>25102366</v>
-      </c>
-      <c r="P35" t="n">
-        <v>11398418.16602279</v>
+      <c r="O35" t="s">
+        <v>31</v>
+      </c>
+      <c r="P35" t="s">
+        <v>31</v>
       </c>
       <c r="Q35" t="n">
         <v>0</v>
       </c>
       <c r="R35" t="n">
-        <v>47363544.11</v>
+        <v>0</v>
       </c>
       <c r="S35" t="n">
-        <v>114409366.4366647</v>
+        <v>0</v>
       </c>
       <c r="T35" t="n">
-        <v>108517521.6629639</v>
+        <v>0</v>
       </c>
       <c r="U35" t="n">
         <v>0</v>
       </c>
       <c r="V35" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="W35" t="s">
         <v>31</v>
@@ -3599,13 +3565,13 @@
         <v>0</v>
       </c>
       <c r="Z35" t="n">
-        <v>14615795.0346875</v>
+        <v>0</v>
       </c>
       <c r="AA35" t="n">
         <v>0</v>
       </c>
       <c r="AB35" t="n">
-        <v>1656178648</v>
+        <v>0</v>
       </c>
       <c r="AC35" t="n">
         <v>0</v>
@@ -3624,78 +3590,40 @@
       <c r="D36" t="s">
         <v>35</v>
       </c>
-      <c r="E36" t="n">
-        <v>1500000</v>
-      </c>
-      <c r="F36" t="s">
-        <v>31</v>
-      </c>
-      <c r="G36" t="s">
-        <v>31</v>
-      </c>
-      <c r="H36" t="n">
-        <v>43500000</v>
-      </c>
-      <c r="I36" t="n">
-        <v>43500000</v>
-      </c>
+      <c r="E36" t="s"/>
+      <c r="F36" t="s"/>
+      <c r="G36" t="s"/>
+      <c r="H36" t="s"/>
+      <c r="I36" t="s"/>
       <c r="J36" t="s"/>
-      <c r="K36" t="n">
-        <v>3000000</v>
-      </c>
-      <c r="L36" t="n">
-        <v>87000000</v>
-      </c>
-      <c r="M36" t="n">
-        <v>87000000</v>
-      </c>
-      <c r="N36" t="s">
-        <v>31</v>
-      </c>
-      <c r="O36" t="n">
-        <v>346262310.92</v>
-      </c>
-      <c r="P36" t="n">
-        <v>89386189.13418086</v>
-      </c>
+      <c r="K36" t="s"/>
+      <c r="L36" t="s"/>
+      <c r="M36" t="s"/>
+      <c r="N36" t="s"/>
+      <c r="O36" t="s"/>
+      <c r="P36" t="s"/>
       <c r="Q36" t="n">
-        <v>238404313.7499999</v>
-      </c>
-      <c r="R36" t="n">
-        <v>247644312.7499999</v>
-      </c>
-      <c r="S36" t="n">
-        <v>419074503.0106418</v>
-      </c>
-      <c r="T36" t="n">
-        <v>401188744.2458702</v>
-      </c>
-      <c r="U36" t="n">
-        <v>32</v>
-      </c>
-      <c r="V36" t="n">
-        <v>0</v>
-      </c>
-      <c r="W36" t="s">
-        <v>31</v>
-      </c>
-      <c r="X36" t="n">
-        <v>261</v>
-      </c>
-      <c r="Y36" t="n">
-        <v>32</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R36" t="s"/>
+      <c r="S36" t="s"/>
+      <c r="T36" t="s"/>
+      <c r="U36" t="s"/>
+      <c r="V36" t="s"/>
+      <c r="W36" t="s"/>
+      <c r="X36" t="s"/>
+      <c r="Y36" t="s"/>
       <c r="Z36" t="n">
         <v>0</v>
       </c>
       <c r="AA36" t="n">
-        <v>4407461536.211874</v>
+        <v>0</v>
       </c>
       <c r="AB36" t="n">
         <v>0</v>
       </c>
       <c r="AC36" t="n">
-        <v>1887615437.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:29">
@@ -3721,10 +3649,10 @@
         <v>31</v>
       </c>
       <c r="H37" t="n">
-        <v>76800000</v>
+        <v>341050000</v>
       </c>
       <c r="I37" t="n">
-        <v>76800000</v>
+        <v>341050000</v>
       </c>
       <c r="J37" t="s">
         <v>31</v>
@@ -3733,58 +3661,58 @@
         <v>4000000</v>
       </c>
       <c r="L37" t="n">
-        <v>153600000</v>
+        <v>682100000</v>
       </c>
       <c r="M37" t="n">
-        <v>153600000</v>
-      </c>
-      <c r="N37" t="s">
-        <v>31</v>
+        <v>682100000</v>
+      </c>
+      <c r="N37" t="n">
+        <v>341050000</v>
       </c>
       <c r="O37" t="n">
-        <v>150506505.58</v>
+        <v>415901572.28</v>
       </c>
       <c r="P37" t="n">
-        <v>90344830.77271318</v>
+        <v>281700432.0429804</v>
       </c>
       <c r="Q37" t="n">
-        <v>1091200393.28</v>
+        <v>1231882238.22</v>
       </c>
       <c r="R37" t="n">
-        <v>1873395544.07</v>
+        <v>2198469355.610001</v>
       </c>
       <c r="S37" t="n">
-        <v>2228444792.571614</v>
+        <v>2513224563.499913</v>
       </c>
       <c r="T37" t="n">
-        <v>2051813150.613717</v>
+        <v>2349927191.849818</v>
       </c>
       <c r="U37" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="V37" t="n">
         <v>0</v>
       </c>
-      <c r="W37" t="s">
-        <v>31</v>
+      <c r="W37" t="n">
+        <v>0</v>
       </c>
       <c r="X37" t="n">
-        <v>76222</v>
+        <v>42775</v>
       </c>
       <c r="Y37" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Z37" t="n">
         <v>0</v>
       </c>
       <c r="AA37" t="n">
-        <v>2220910151.515152</v>
+        <v>3412149206.349206</v>
       </c>
       <c r="AB37" t="n">
         <v>0</v>
       </c>
       <c r="AC37" t="n">
-        <v>13561083827.29927</v>
+        <v>16735799835.25</v>
       </c>
     </row>
     <row r="38" spans="1:29">
@@ -3810,10 +3738,10 @@
         <v>31</v>
       </c>
       <c r="H38" t="n">
-        <v>29000000</v>
+        <v>28000000</v>
       </c>
       <c r="I38" t="n">
-        <v>29000000</v>
+        <v>28000000</v>
       </c>
       <c r="J38" t="s">
         <v>31</v>
@@ -3822,58 +3750,58 @@
         <v>2000000</v>
       </c>
       <c r="L38" t="n">
-        <v>58000000</v>
+        <v>56000000</v>
       </c>
       <c r="M38" t="n">
-        <v>58000000</v>
-      </c>
-      <c r="N38" t="s">
-        <v>31</v>
+        <v>56000000</v>
+      </c>
+      <c r="N38" t="n">
+        <v>28000000</v>
       </c>
       <c r="O38" t="n">
-        <v>88422424.87</v>
+        <v>83624817.22999999</v>
       </c>
       <c r="P38" t="n">
-        <v>42428035.33703334</v>
+        <v>22918862.46031372</v>
       </c>
       <c r="Q38" t="n">
-        <v>0</v>
+        <v>2116247.92</v>
       </c>
       <c r="R38" t="n">
-        <v>1457925934.91</v>
+        <v>1291836830.6</v>
       </c>
       <c r="S38" t="n">
-        <v>1976919480.460715</v>
+        <v>1775456383.446402</v>
       </c>
       <c r="T38" t="n">
-        <v>1946463163.84877</v>
+        <v>1730858382.008108</v>
       </c>
       <c r="U38" t="n">
         <v>0</v>
       </c>
       <c r="V38" t="n">
-        <v>30</v>
-      </c>
-      <c r="W38" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="W38" t="n">
+        <v>0</v>
       </c>
       <c r="X38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z38" t="n">
         <v>0</v>
       </c>
       <c r="AA38" t="n">
-        <v>2960630848.274603</v>
+        <v>2147561134.778922</v>
       </c>
       <c r="AB38" t="n">
         <v>0</v>
       </c>
       <c r="AC38" t="n">
-        <v>22074909141.00999</v>
+        <v>17868539938.52748</v>
       </c>
     </row>
     <row r="39" spans="1:29">
@@ -3899,10 +3827,10 @@
         <v>31</v>
       </c>
       <c r="H39" t="n">
-        <v>11000000</v>
+        <v>13200000</v>
       </c>
       <c r="I39" t="n">
-        <v>11000000</v>
+        <v>13200000</v>
       </c>
       <c r="J39" t="s">
         <v>31</v>
@@ -3911,31 +3839,31 @@
         <v>1000000</v>
       </c>
       <c r="L39" t="n">
-        <v>22000000</v>
+        <v>26400000</v>
       </c>
       <c r="M39" t="n">
-        <v>22000000</v>
-      </c>
-      <c r="N39" t="s">
-        <v>31</v>
+        <v>26400000</v>
+      </c>
+      <c r="N39" t="n">
+        <v>13200000</v>
       </c>
       <c r="O39" t="n">
-        <v>14280575.65</v>
+        <v>16185622.88</v>
       </c>
       <c r="P39" t="n">
-        <v>10905990.35294574</v>
+        <v>11314466.51141176</v>
       </c>
       <c r="Q39" t="n">
-        <v>45669342.05</v>
+        <v>79033552.61</v>
       </c>
       <c r="R39" t="n">
-        <v>46690696.62</v>
+        <v>79033552.61</v>
       </c>
       <c r="S39" t="n">
-        <v>51790867.2718074</v>
+        <v>78909861.05337371</v>
       </c>
       <c r="T39" t="n">
-        <v>50875850.859403</v>
+        <v>78732192.92559727</v>
       </c>
       <c r="U39" t="n">
         <v>6</v>
@@ -3943,11 +3871,11 @@
       <c r="V39" t="n">
         <v>0</v>
       </c>
-      <c r="W39" t="s">
-        <v>31</v>
+      <c r="W39" t="n">
+        <v>0</v>
       </c>
       <c r="X39" t="n">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="Y39" t="n">
         <v>6</v>
@@ -3956,13 +3884,13 @@
         <v>0</v>
       </c>
       <c r="AA39" t="n">
-        <v>4904907.748181818</v>
+        <v>2627670.127619048</v>
       </c>
       <c r="AB39" t="n">
         <v>0</v>
       </c>
       <c r="AC39" t="n">
-        <v>377751937.3800001</v>
+        <v>490426526.1749998</v>
       </c>
     </row>
     <row r="40" spans="1:29">
@@ -3988,10 +3916,10 @@
         <v>31</v>
       </c>
       <c r="H40" t="n">
-        <v>13050000</v>
+        <v>8000000</v>
       </c>
       <c r="I40" t="n">
-        <v>13050000</v>
+        <v>8000000</v>
       </c>
       <c r="J40" t="s">
         <v>31</v>
@@ -4000,31 +3928,31 @@
         <v>2000000</v>
       </c>
       <c r="L40" t="n">
-        <v>26100000</v>
+        <v>16000000</v>
       </c>
       <c r="M40" t="n">
-        <v>26100000</v>
-      </c>
-      <c r="N40" t="s">
-        <v>31</v>
+        <v>16000000</v>
+      </c>
+      <c r="N40" t="n">
+        <v>8000000</v>
       </c>
       <c r="O40" t="n">
-        <v>25102366</v>
+        <v>15905959.9772</v>
       </c>
       <c r="P40" t="n">
-        <v>8218754.290567633</v>
+        <v>8481269.385170585</v>
       </c>
       <c r="Q40" t="n">
         <v>0</v>
       </c>
       <c r="R40" t="n">
-        <v>53993946.26</v>
+        <v>7959389.49</v>
       </c>
       <c r="S40" t="n">
-        <v>70606084.92640869</v>
+        <v>31962562.32236112</v>
       </c>
       <c r="T40" t="n">
-        <v>68618283.86456735</v>
+        <v>30198249.05959623</v>
       </c>
       <c r="U40" t="n">
         <v>0</v>
@@ -4032,8 +3960,8 @@
       <c r="V40" t="n">
         <v>9</v>
       </c>
-      <c r="W40" t="s">
-        <v>31</v>
+      <c r="W40" t="n">
+        <v>0</v>
       </c>
       <c r="X40" t="n">
         <v>0</v>
@@ -4042,13 +3970,13 @@
         <v>0</v>
       </c>
       <c r="Z40" t="n">
-        <v>23966156.01515152</v>
+        <v>24825396.82539682</v>
       </c>
       <c r="AA40" t="n">
         <v>0</v>
       </c>
       <c r="AB40" t="n">
-        <v>2669166297</v>
+        <v>469913313.8699999</v>
       </c>
       <c r="AC40" t="n">
         <v>0</v>
@@ -4077,68 +4005,70 @@
         <v>31</v>
       </c>
       <c r="H41" t="n">
-        <v>81950000</v>
+        <v>88250000</v>
       </c>
       <c r="I41" t="n">
-        <v>81950000</v>
-      </c>
-      <c r="J41" t="s"/>
+        <v>88250000</v>
+      </c>
+      <c r="J41" t="s">
+        <v>31</v>
+      </c>
       <c r="K41" t="n">
         <v>3000000</v>
       </c>
       <c r="L41" t="n">
-        <v>163900000</v>
+        <v>176500000</v>
       </c>
       <c r="M41" t="n">
-        <v>163900000</v>
-      </c>
-      <c r="N41" t="s">
-        <v>31</v>
+        <v>176500000</v>
+      </c>
+      <c r="N41" t="n">
+        <v>88250000</v>
       </c>
       <c r="O41" t="n">
-        <v>346262310.92</v>
+        <v>749432256</v>
       </c>
       <c r="P41" t="n">
-        <v>94313396.50398234</v>
+        <v>127219022.2716863</v>
       </c>
       <c r="Q41" t="n">
-        <v>492225962.6</v>
+        <v>198285453.89</v>
       </c>
       <c r="R41" t="n">
-        <v>518900008</v>
+        <v>202904762.5700001</v>
       </c>
       <c r="S41" t="n">
-        <v>533130691.1440281</v>
+        <v>424144037.7920223</v>
       </c>
       <c r="T41" t="n">
-        <v>519780277.0735425</v>
+        <v>404341742.3368806</v>
       </c>
       <c r="U41" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="V41" t="n">
-        <v>12</v>
-      </c>
-      <c r="W41" t="s">
-        <v>31</v>
+        <v>0</v>
+      </c>
+      <c r="W41" t="n">
+        <v>0</v>
       </c>
       <c r="X41" t="n">
-        <v>214</v>
+        <v>258</v>
       </c>
       <c r="Y41" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="Z41" t="n">
         <v>0</v>
       </c>
       <c r="AA41" t="n">
-        <v>3598081239.559697</v>
+        <v>4983780341.471429</v>
       </c>
       <c r="AB41" t="n">
         <v>0</v>
       </c>
       <c r="AC41" t="n">
-        <v>4191887515.43</v>
+        <v>1835750898.48</v>
       </c>
     </row>
     <row r="42" spans="1:29">
@@ -4164,10 +4094,10 @@
         <v>31</v>
       </c>
       <c r="H42" t="n">
-        <v>384150000</v>
+        <v>65250000</v>
       </c>
       <c r="I42" t="n">
-        <v>384150000</v>
+        <v>65250000</v>
       </c>
       <c r="J42" t="s">
         <v>31</v>
@@ -4176,58 +4106,58 @@
         <v>4000000</v>
       </c>
       <c r="L42" t="n">
-        <v>768300000</v>
+        <v>130500000</v>
       </c>
       <c r="M42" t="n">
-        <v>768300000</v>
-      </c>
-      <c r="N42" t="n">
-        <v>384150000</v>
+        <v>130500000</v>
+      </c>
+      <c r="N42" t="s">
+        <v>31</v>
       </c>
       <c r="O42" t="n">
-        <v>428460956.6</v>
+        <v>128575078.3</v>
       </c>
       <c r="P42" t="n">
-        <v>332139280.1247033</v>
+        <v>85784721.51953307</v>
       </c>
       <c r="Q42" t="n">
-        <v>782102567.4200001</v>
+        <v>944508985.3000001</v>
       </c>
       <c r="R42" t="n">
-        <v>1968950195.79</v>
+        <v>1615585684.27</v>
       </c>
       <c r="S42" t="n">
-        <v>2221556815.099343</v>
+        <v>2122726809.248829</v>
       </c>
       <c r="T42" t="n">
-        <v>2069278190.65994</v>
+        <v>1919778423.562241</v>
       </c>
       <c r="U42" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V42" t="n">
         <v>0</v>
       </c>
-      <c r="W42" t="n">
-        <v>0</v>
+      <c r="W42" t="s">
+        <v>31</v>
       </c>
       <c r="X42" t="n">
-        <v>41954</v>
+        <v>76593</v>
       </c>
       <c r="Y42" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Z42" t="n">
         <v>0</v>
       </c>
       <c r="AA42" t="n">
-        <v>3012736825.396825</v>
+        <v>2526057656.25</v>
       </c>
       <c r="AB42" t="n">
         <v>0</v>
       </c>
       <c r="AC42" t="n">
-        <v>16008711084.54</v>
+        <v>12295069331.51122</v>
       </c>
     </row>
     <row r="43" spans="1:29">
@@ -4253,10 +4183,10 @@
         <v>31</v>
       </c>
       <c r="H43" t="n">
-        <v>27000000</v>
+        <v>29000000</v>
       </c>
       <c r="I43" t="n">
-        <v>27000000</v>
+        <v>29000000</v>
       </c>
       <c r="J43" t="s">
         <v>31</v>
@@ -4265,58 +4195,58 @@
         <v>2000000</v>
       </c>
       <c r="L43" t="n">
-        <v>54000000</v>
+        <v>58000000</v>
       </c>
       <c r="M43" t="n">
-        <v>54000000</v>
-      </c>
-      <c r="N43" t="n">
-        <v>27000000</v>
+        <v>58000000</v>
+      </c>
+      <c r="N43" t="s">
+        <v>31</v>
       </c>
       <c r="O43" t="n">
-        <v>59546943.39</v>
+        <v>77564196.22</v>
       </c>
       <c r="P43" t="n">
-        <v>20219182.21703557</v>
+        <v>33825150.34933851</v>
       </c>
       <c r="Q43" t="n">
-        <v>9163237.48</v>
+        <v>0</v>
       </c>
       <c r="R43" t="n">
-        <v>1632725579.19</v>
+        <v>1081511424.12</v>
       </c>
       <c r="S43" t="n">
-        <v>1816055702.907279</v>
+        <v>1633609837.239741</v>
       </c>
       <c r="T43" t="n">
-        <v>1785347553.849961</v>
+        <v>1601753380.477004</v>
       </c>
       <c r="U43" t="n">
         <v>0</v>
       </c>
       <c r="V43" t="n">
-        <v>27</v>
-      </c>
-      <c r="W43" t="n">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="W43" t="s">
+        <v>31</v>
       </c>
       <c r="X43" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="Y43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z43" t="n">
         <v>0</v>
       </c>
       <c r="AA43" t="n">
-        <v>1125482237.542957</v>
+        <v>3018566648.816501</v>
       </c>
       <c r="AB43" t="n">
         <v>0</v>
       </c>
       <c r="AC43" t="n">
-        <v>12812299707.18952</v>
+        <v>17203359798.564</v>
       </c>
     </row>
     <row r="44" spans="1:29">
@@ -4342,10 +4272,10 @@
         <v>31</v>
       </c>
       <c r="H44" t="n">
-        <v>11600000</v>
+        <v>10000000</v>
       </c>
       <c r="I44" t="n">
-        <v>11600000</v>
+        <v>10000000</v>
       </c>
       <c r="J44" t="s">
         <v>31</v>
@@ -4354,31 +4284,31 @@
         <v>1000000</v>
       </c>
       <c r="L44" t="n">
-        <v>23200000</v>
+        <v>20000000</v>
       </c>
       <c r="M44" t="n">
-        <v>23200000</v>
-      </c>
-      <c r="N44" t="n">
-        <v>11600000</v>
+        <v>20000000</v>
+      </c>
+      <c r="N44" t="s">
+        <v>31</v>
       </c>
       <c r="O44" t="n">
-        <v>16185622.88</v>
+        <v>21539150.61</v>
       </c>
       <c r="P44" t="n">
-        <v>11624850.99849802</v>
+        <v>12919611.23412452</v>
       </c>
       <c r="Q44" t="n">
-        <v>54615555.88</v>
+        <v>60522636.47</v>
       </c>
       <c r="R44" t="n">
-        <v>54615555.88</v>
+        <v>61018440.4</v>
       </c>
       <c r="S44" t="n">
-        <v>53269965.77986963</v>
+        <v>67315060.94766967</v>
       </c>
       <c r="T44" t="n">
-        <v>53142015.74525239</v>
+        <v>66250545.85192169</v>
       </c>
       <c r="U44" t="n">
         <v>6</v>
@@ -4386,11 +4316,11 @@
       <c r="V44" t="n">
         <v>0</v>
       </c>
-      <c r="W44" t="n">
-        <v>0</v>
+      <c r="W44" t="s">
+        <v>31</v>
       </c>
       <c r="X44" t="n">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="Y44" t="n">
         <v>6</v>
@@ -4399,13 +4329,13 @@
         <v>0</v>
       </c>
       <c r="AA44" t="n">
-        <v>1991447.398730159</v>
+        <v>4910347.617656251</v>
       </c>
       <c r="AB44" t="n">
         <v>0</v>
       </c>
       <c r="AC44" t="n">
-        <v>364949939.2049998</v>
+        <v>441979282.6799994</v>
       </c>
     </row>
     <row r="45" spans="1:29">
@@ -4431,10 +4361,10 @@
         <v>31</v>
       </c>
       <c r="H45" t="n">
-        <v>8000000</v>
+        <v>19700000</v>
       </c>
       <c r="I45" t="n">
-        <v>8000000</v>
+        <v>19700000</v>
       </c>
       <c r="J45" t="s">
         <v>31</v>
@@ -4443,31 +4373,31 @@
         <v>2000000</v>
       </c>
       <c r="L45" t="n">
-        <v>16000000</v>
+        <v>39400000</v>
       </c>
       <c r="M45" t="n">
-        <v>16000000</v>
-      </c>
-      <c r="N45" t="n">
-        <v>8000000</v>
+        <v>39400000</v>
+      </c>
+      <c r="N45" t="s">
+        <v>31</v>
       </c>
       <c r="O45" t="n">
-        <v>9661830.854600001</v>
+        <v>25102366</v>
       </c>
       <c r="P45" t="n">
-        <v>6339617.495558105</v>
+        <v>11398418.16602279</v>
       </c>
       <c r="Q45" t="n">
         <v>0</v>
       </c>
       <c r="R45" t="n">
-        <v>8996543.780000001</v>
+        <v>47363544.11</v>
       </c>
       <c r="S45" t="n">
-        <v>35441064.51149503</v>
+        <v>114409366.4366647</v>
       </c>
       <c r="T45" t="n">
-        <v>33365849.88093312</v>
+        <v>108517521.6629639</v>
       </c>
       <c r="U45" t="n">
         <v>0</v>
@@ -4475,8 +4405,8 @@
       <c r="V45" t="n">
         <v>9</v>
       </c>
-      <c r="W45" t="n">
-        <v>0</v>
+      <c r="W45" t="s">
+        <v>31</v>
       </c>
       <c r="X45" t="n">
         <v>0</v>
@@ -4485,13 +4415,13 @@
         <v>0</v>
       </c>
       <c r="Z45" t="n">
-        <v>235358.6676190476</v>
+        <v>14615795.0346875</v>
       </c>
       <c r="AA45" t="n">
         <v>0</v>
       </c>
       <c r="AB45" t="n">
-        <v>484740909.9299998</v>
+        <v>1656178648</v>
       </c>
       <c r="AC45" t="n">
         <v>0</v>
@@ -4520,69 +4450,955 @@
         <v>31</v>
       </c>
       <c r="H46" t="n">
-        <v>93250000</v>
+        <v>43500000</v>
       </c>
       <c r="I46" t="n">
-        <v>93250000</v>
-      </c>
-      <c r="J46" t="s">
-        <v>31</v>
-      </c>
+        <v>43500000</v>
+      </c>
+      <c r="J46" t="s"/>
       <c r="K46" t="n">
         <v>3000000</v>
       </c>
       <c r="L46" t="n">
+        <v>87000000</v>
+      </c>
+      <c r="M46" t="n">
+        <v>87000000</v>
+      </c>
+      <c r="N46" t="s">
+        <v>31</v>
+      </c>
+      <c r="O46" t="n">
+        <v>346262310.92</v>
+      </c>
+      <c r="P46" t="n">
+        <v>89386189.13418086</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>238404313.7499999</v>
+      </c>
+      <c r="R46" t="n">
+        <v>247644312.7499999</v>
+      </c>
+      <c r="S46" t="n">
+        <v>419074503.0106418</v>
+      </c>
+      <c r="T46" t="n">
+        <v>401188744.2458702</v>
+      </c>
+      <c r="U46" t="n">
+        <v>32</v>
+      </c>
+      <c r="V46" t="n">
+        <v>0</v>
+      </c>
+      <c r="W46" t="s">
+        <v>31</v>
+      </c>
+      <c r="X46" t="n">
+        <v>261</v>
+      </c>
+      <c r="Y46" t="n">
+        <v>32</v>
+      </c>
+      <c r="Z46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA46" t="n">
+        <v>4407461536.211874</v>
+      </c>
+      <c r="AB46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC46" t="n">
+        <v>1887615437.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="F47" t="s">
+        <v>31</v>
+      </c>
+      <c r="G47" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" t="n">
+        <v>76800000</v>
+      </c>
+      <c r="I47" t="n">
+        <v>76800000</v>
+      </c>
+      <c r="J47" t="s">
+        <v>31</v>
+      </c>
+      <c r="K47" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="L47" t="n">
+        <v>153600000</v>
+      </c>
+      <c r="M47" t="n">
+        <v>153600000</v>
+      </c>
+      <c r="N47" t="s">
+        <v>31</v>
+      </c>
+      <c r="O47" t="n">
+        <v>150506505.58</v>
+      </c>
+      <c r="P47" t="n">
+        <v>90344830.77271318</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>1091200393.28</v>
+      </c>
+      <c r="R47" t="n">
+        <v>1873395544.07</v>
+      </c>
+      <c r="S47" t="n">
+        <v>2228444792.571614</v>
+      </c>
+      <c r="T47" t="n">
+        <v>2051813150.613717</v>
+      </c>
+      <c r="U47" t="n">
+        <v>36</v>
+      </c>
+      <c r="V47" t="n">
+        <v>0</v>
+      </c>
+      <c r="W47" t="s">
+        <v>31</v>
+      </c>
+      <c r="X47" t="n">
+        <v>76222</v>
+      </c>
+      <c r="Y47" t="n">
+        <v>36</v>
+      </c>
+      <c r="Z47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA47" t="n">
+        <v>2220910151.515152</v>
+      </c>
+      <c r="AB47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC47" t="n">
+        <v>13561083827.29927</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="F48" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" t="s">
+        <v>31</v>
+      </c>
+      <c r="H48" t="n">
+        <v>29000000</v>
+      </c>
+      <c r="I48" t="n">
+        <v>29000000</v>
+      </c>
+      <c r="J48" t="s">
+        <v>31</v>
+      </c>
+      <c r="K48" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="L48" t="n">
+        <v>58000000</v>
+      </c>
+      <c r="M48" t="n">
+        <v>58000000</v>
+      </c>
+      <c r="N48" t="s">
+        <v>31</v>
+      </c>
+      <c r="O48" t="n">
+        <v>88422424.87</v>
+      </c>
+      <c r="P48" t="n">
+        <v>42428035.33703334</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0</v>
+      </c>
+      <c r="R48" t="n">
+        <v>1457925934.91</v>
+      </c>
+      <c r="S48" t="n">
+        <v>1976919480.460715</v>
+      </c>
+      <c r="T48" t="n">
+        <v>1946463163.84877</v>
+      </c>
+      <c r="U48" t="n">
+        <v>0</v>
+      </c>
+      <c r="V48" t="n">
+        <v>30</v>
+      </c>
+      <c r="W48" t="s">
+        <v>31</v>
+      </c>
+      <c r="X48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA48" t="n">
+        <v>2960630848.274603</v>
+      </c>
+      <c r="AB48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC48" t="n">
+        <v>22074909141.00999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" t="n">
+        <v>500000</v>
+      </c>
+      <c r="F49" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" t="n">
+        <v>11000000</v>
+      </c>
+      <c r="I49" t="n">
+        <v>11000000</v>
+      </c>
+      <c r="J49" t="s">
+        <v>31</v>
+      </c>
+      <c r="K49" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="L49" t="n">
+        <v>22000000</v>
+      </c>
+      <c r="M49" t="n">
+        <v>22000000</v>
+      </c>
+      <c r="N49" t="s">
+        <v>31</v>
+      </c>
+      <c r="O49" t="n">
+        <v>14280575.65</v>
+      </c>
+      <c r="P49" t="n">
+        <v>10905990.35294574</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>45669342.05</v>
+      </c>
+      <c r="R49" t="n">
+        <v>46690696.62</v>
+      </c>
+      <c r="S49" t="n">
+        <v>51790867.2718074</v>
+      </c>
+      <c r="T49" t="n">
+        <v>50875850.859403</v>
+      </c>
+      <c r="U49" t="n">
+        <v>6</v>
+      </c>
+      <c r="V49" t="n">
+        <v>0</v>
+      </c>
+      <c r="W49" t="s">
+        <v>31</v>
+      </c>
+      <c r="X49" t="n">
+        <v>130</v>
+      </c>
+      <c r="Y49" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z49" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA49" t="n">
+        <v>4904907.748181818</v>
+      </c>
+      <c r="AB49" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC49" t="n">
+        <v>377751937.3800001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="F50" t="s">
+        <v>31</v>
+      </c>
+      <c r="G50" t="s">
+        <v>31</v>
+      </c>
+      <c r="H50" t="n">
+        <v>13050000</v>
+      </c>
+      <c r="I50" t="n">
+        <v>13050000</v>
+      </c>
+      <c r="J50" t="s">
+        <v>31</v>
+      </c>
+      <c r="K50" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="L50" t="n">
+        <v>26100000</v>
+      </c>
+      <c r="M50" t="n">
+        <v>26100000</v>
+      </c>
+      <c r="N50" t="s">
+        <v>31</v>
+      </c>
+      <c r="O50" t="n">
+        <v>25102366</v>
+      </c>
+      <c r="P50" t="n">
+        <v>8218754.290567633</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>0</v>
+      </c>
+      <c r="R50" t="n">
+        <v>53993946.26</v>
+      </c>
+      <c r="S50" t="n">
+        <v>70606084.92640869</v>
+      </c>
+      <c r="T50" t="n">
+        <v>68618283.86456735</v>
+      </c>
+      <c r="U50" t="n">
+        <v>0</v>
+      </c>
+      <c r="V50" t="n">
+        <v>9</v>
+      </c>
+      <c r="W50" t="s">
+        <v>31</v>
+      </c>
+      <c r="X50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z50" t="n">
+        <v>23966156.01515152</v>
+      </c>
+      <c r="AA50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB50" t="n">
+        <v>2669166297</v>
+      </c>
+      <c r="AC50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" t="s">
+        <v>44</v>
+      </c>
+      <c r="D51" t="s">
+        <v>35</v>
+      </c>
+      <c r="E51" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="F51" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" t="n">
+        <v>81950000</v>
+      </c>
+      <c r="I51" t="n">
+        <v>81950000</v>
+      </c>
+      <c r="J51" t="s"/>
+      <c r="K51" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="L51" t="n">
+        <v>163900000</v>
+      </c>
+      <c r="M51" t="n">
+        <v>163900000</v>
+      </c>
+      <c r="N51" t="s">
+        <v>31</v>
+      </c>
+      <c r="O51" t="n">
+        <v>346262310.92</v>
+      </c>
+      <c r="P51" t="n">
+        <v>94313396.50398234</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>492225962.6</v>
+      </c>
+      <c r="R51" t="n">
+        <v>518900008</v>
+      </c>
+      <c r="S51" t="n">
+        <v>533130691.1440281</v>
+      </c>
+      <c r="T51" t="n">
+        <v>519780277.0735425</v>
+      </c>
+      <c r="U51" t="n">
+        <v>22</v>
+      </c>
+      <c r="V51" t="n">
+        <v>12</v>
+      </c>
+      <c r="W51" t="s">
+        <v>31</v>
+      </c>
+      <c r="X51" t="n">
+        <v>214</v>
+      </c>
+      <c r="Y51" t="n">
+        <v>22</v>
+      </c>
+      <c r="Z51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA51" t="n">
+        <v>3598081239.559697</v>
+      </c>
+      <c r="AB51" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC51" t="n">
+        <v>4191887515.43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="F52" t="s">
+        <v>31</v>
+      </c>
+      <c r="G52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H52" t="n">
+        <v>384150000</v>
+      </c>
+      <c r="I52" t="n">
+        <v>384150000</v>
+      </c>
+      <c r="J52" t="s">
+        <v>31</v>
+      </c>
+      <c r="K52" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="L52" t="n">
+        <v>768300000</v>
+      </c>
+      <c r="M52" t="n">
+        <v>768300000</v>
+      </c>
+      <c r="N52" t="n">
+        <v>384150000</v>
+      </c>
+      <c r="O52" t="n">
+        <v>428460956.6</v>
+      </c>
+      <c r="P52" t="n">
+        <v>332139280.1247033</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>782102567.4200001</v>
+      </c>
+      <c r="R52" t="n">
+        <v>1968950195.79</v>
+      </c>
+      <c r="S52" t="n">
+        <v>2221556815.099343</v>
+      </c>
+      <c r="T52" t="n">
+        <v>2069278190.65994</v>
+      </c>
+      <c r="U52" t="n">
+        <v>36</v>
+      </c>
+      <c r="V52" t="n">
+        <v>0</v>
+      </c>
+      <c r="W52" t="n">
+        <v>0</v>
+      </c>
+      <c r="X52" t="n">
+        <v>41954</v>
+      </c>
+      <c r="Y52" t="n">
+        <v>33</v>
+      </c>
+      <c r="Z52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA52" t="n">
+        <v>3012736825.396825</v>
+      </c>
+      <c r="AB52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC52" t="n">
+        <v>16008711084.54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="F53" t="s">
+        <v>31</v>
+      </c>
+      <c r="G53" t="s">
+        <v>31</v>
+      </c>
+      <c r="H53" t="n">
+        <v>27000000</v>
+      </c>
+      <c r="I53" t="n">
+        <v>27000000</v>
+      </c>
+      <c r="J53" t="s">
+        <v>31</v>
+      </c>
+      <c r="K53" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="L53" t="n">
+        <v>54000000</v>
+      </c>
+      <c r="M53" t="n">
+        <v>54000000</v>
+      </c>
+      <c r="N53" t="n">
+        <v>27000000</v>
+      </c>
+      <c r="O53" t="n">
+        <v>59546943.39</v>
+      </c>
+      <c r="P53" t="n">
+        <v>20219182.21703557</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>9163237.48</v>
+      </c>
+      <c r="R53" t="n">
+        <v>1632725579.19</v>
+      </c>
+      <c r="S53" t="n">
+        <v>1816055702.907279</v>
+      </c>
+      <c r="T53" t="n">
+        <v>1785347553.849961</v>
+      </c>
+      <c r="U53" t="n">
+        <v>0</v>
+      </c>
+      <c r="V53" t="n">
+        <v>27</v>
+      </c>
+      <c r="W53" t="n">
+        <v>0</v>
+      </c>
+      <c r="X53" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y53" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA53" t="n">
+        <v>1125482237.542957</v>
+      </c>
+      <c r="AB53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC53" t="n">
+        <v>12812299707.18952</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" t="s">
+        <v>45</v>
+      </c>
+      <c r="D54" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" t="n">
+        <v>500000</v>
+      </c>
+      <c r="F54" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" t="s">
+        <v>31</v>
+      </c>
+      <c r="H54" t="n">
+        <v>11600000</v>
+      </c>
+      <c r="I54" t="n">
+        <v>11600000</v>
+      </c>
+      <c r="J54" t="s">
+        <v>31</v>
+      </c>
+      <c r="K54" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="L54" t="n">
+        <v>23200000</v>
+      </c>
+      <c r="M54" t="n">
+        <v>23200000</v>
+      </c>
+      <c r="N54" t="n">
+        <v>11600000</v>
+      </c>
+      <c r="O54" t="n">
+        <v>16185622.88</v>
+      </c>
+      <c r="P54" t="n">
+        <v>11624850.99849802</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>54615555.88</v>
+      </c>
+      <c r="R54" t="n">
+        <v>54615555.88</v>
+      </c>
+      <c r="S54" t="n">
+        <v>53269965.77986963</v>
+      </c>
+      <c r="T54" t="n">
+        <v>53142015.74525239</v>
+      </c>
+      <c r="U54" t="n">
+        <v>6</v>
+      </c>
+      <c r="V54" t="n">
+        <v>0</v>
+      </c>
+      <c r="W54" t="n">
+        <v>0</v>
+      </c>
+      <c r="X54" t="n">
+        <v>123</v>
+      </c>
+      <c r="Y54" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA54" t="n">
+        <v>1991447.398730159</v>
+      </c>
+      <c r="AB54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC54" t="n">
+        <v>364949939.2049998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="F55" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" t="s">
+        <v>31</v>
+      </c>
+      <c r="H55" t="n">
+        <v>8000000</v>
+      </c>
+      <c r="I55" t="n">
+        <v>8000000</v>
+      </c>
+      <c r="J55" t="s">
+        <v>31</v>
+      </c>
+      <c r="K55" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="L55" t="n">
+        <v>16000000</v>
+      </c>
+      <c r="M55" t="n">
+        <v>16000000</v>
+      </c>
+      <c r="N55" t="n">
+        <v>8000000</v>
+      </c>
+      <c r="O55" t="n">
+        <v>9661830.854600001</v>
+      </c>
+      <c r="P55" t="n">
+        <v>6339617.495558105</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>0</v>
+      </c>
+      <c r="R55" t="n">
+        <v>8996543.780000001</v>
+      </c>
+      <c r="S55" t="n">
+        <v>35441064.51149503</v>
+      </c>
+      <c r="T55" t="n">
+        <v>33365849.88093312</v>
+      </c>
+      <c r="U55" t="n">
+        <v>0</v>
+      </c>
+      <c r="V55" t="n">
+        <v>9</v>
+      </c>
+      <c r="W55" t="n">
+        <v>0</v>
+      </c>
+      <c r="X55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z55" t="n">
+        <v>235358.6676190476</v>
+      </c>
+      <c r="AA55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB55" t="n">
+        <v>484740909.9299998</v>
+      </c>
+      <c r="AC55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" t="s">
+        <v>45</v>
+      </c>
+      <c r="D56" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="F56" t="s">
+        <v>31</v>
+      </c>
+      <c r="G56" t="s">
+        <v>31</v>
+      </c>
+      <c r="H56" t="n">
+        <v>93250000</v>
+      </c>
+      <c r="I56" t="n">
+        <v>93250000</v>
+      </c>
+      <c r="J56" t="s">
+        <v>31</v>
+      </c>
+      <c r="K56" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="L56" t="n">
         <v>186500000</v>
       </c>
-      <c r="M46" t="n">
+      <c r="M56" t="n">
         <v>186500000</v>
       </c>
-      <c r="N46" t="n">
+      <c r="N56" t="n">
         <v>93250000</v>
       </c>
-      <c r="O46" t="n">
+      <c r="O56" t="n">
         <v>749432256</v>
       </c>
-      <c r="P46" t="n">
+      <c r="P56" t="n">
         <v>119458165.5448222</v>
       </c>
-      <c r="Q46" t="n">
+      <c r="Q56" t="n">
         <v>249021678.29</v>
       </c>
-      <c r="R46" t="n">
+      <c r="R56" t="n">
         <v>284606755.47</v>
       </c>
-      <c r="S46" t="n">
+      <c r="S56" t="n">
         <v>548505961.4461385</v>
       </c>
-      <c r="T46" t="n">
+      <c r="T56" t="n">
         <v>526219043.3239136</v>
       </c>
-      <c r="U46" t="n">
-        <v>28</v>
-      </c>
-      <c r="V46" t="n">
-        <v>0</v>
-      </c>
-      <c r="W46" t="n">
-        <v>0</v>
-      </c>
-      <c r="X46" t="n">
+      <c r="U56" t="n">
+        <v>28</v>
+      </c>
+      <c r="V56" t="n">
+        <v>0</v>
+      </c>
+      <c r="W56" t="n">
+        <v>0</v>
+      </c>
+      <c r="X56" t="n">
         <v>252</v>
       </c>
-      <c r="Y46" t="n">
+      <c r="Y56" t="n">
         <v>27</v>
       </c>
-      <c r="Z46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA46" t="n">
+      <c r="Z56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA56" t="n">
         <v>4537123266.064445</v>
       </c>
-      <c r="AB46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC46" t="n">
+      <c r="AB56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC56" t="n">
         <v>2637929155.69</v>
       </c>
     </row>

</xml_diff>